<commit_message>
overview / task ill finish up
</commit_message>
<xml_diff>
--- a/Activity Log.xlsx
+++ b/Activity Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rremi\Desktop\ECE 366\Hex-Decoder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rami\Documents\GitHub\Hex-Decoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC77011-203E-49F4-BA04-BD2DCBD1F075}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4947BC67-2911-4A09-8297-E71C5E8831AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5724" yWindow="2892" windowWidth="17280" windowHeight="8964" xr2:uid="{0F5DC705-85FB-4EAC-8F72-74DC7DEA8333}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0F5DC705-85FB-4EAC-8F72-74DC7DEA8333}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Date/Location</t>
   </si>
@@ -73,6 +67,18 @@
   </si>
   <si>
     <t>Fix srl functionality</t>
+  </si>
+  <si>
+    <t>Friday 10:00PM - 12:00 AM</t>
+  </si>
+  <si>
+    <t>Understanding the program</t>
+  </si>
+  <si>
+    <t>Fix and polish certain areas of the test cases</t>
+  </si>
+  <si>
+    <t>Rami</t>
   </si>
 </sst>
 </file>
@@ -438,22 +444,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6CA3FDB-D763-4CE5-9DE9-DF6F5D651576}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="31" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47.19921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.1328125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -467,7 +473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -481,7 +487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -495,7 +501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -507,6 +513,20 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
offset for lw and sw in case 4
</commit_message>
<xml_diff>
--- a/Activity Log.xlsx
+++ b/Activity Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rami\Documents\GitHub\Hex-Decoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4947BC67-2911-4A09-8297-E71C5E8831AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50A3C0E-A584-4D89-88A2-45097801A515}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0F5DC705-85FB-4EAC-8F72-74DC7DEA8333}"/>
   </bookViews>
@@ -69,16 +69,16 @@
     <t>Fix srl functionality</t>
   </si>
   <si>
-    <t>Friday 10:00PM - 12:00 AM</t>
-  </si>
-  <si>
-    <t>Understanding the program</t>
-  </si>
-  <si>
-    <t>Fix and polish certain areas of the test cases</t>
-  </si>
-  <si>
     <t>Rami</t>
+  </si>
+  <si>
+    <t>Satuday 12:00PM - 2:00 PM</t>
+  </si>
+  <si>
+    <t>Understanding the program/ Looking over case 4</t>
+  </si>
+  <si>
+    <t>Fixed offset on Lw and sw instructions. Fixing other potential issues</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
     <col min="2" max="2" width="60" style="1" customWidth="1"/>
-    <col min="3" max="3" width="47.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="34.1328125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.86328125" style="1"/>
   </cols>
@@ -517,16 +517,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>